<commit_message>
Move Central America, Caribbeans CO, GF & VE to NA region
Consider the locations below as NA instead of SA.

GF, VE, CO, GY, SR, GT, HN, CR, PA, CU, DO, HT, JM, GP, PR, LC, DM, BB, MS

Tempfix before implementing a proper Central America region.
</commit_message>
<xml_diff>
--- a/country_continents.xlsx
+++ b/country_continents.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine T\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\UrT-Pickup\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EEC4E8-CF14-447B-8368-0A7A1D7EB4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2351,7 +2352,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -2670,21 +2671,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F263"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="C264" sqref="C264"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3689,10 +3690,10 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C51" t="s">
         <v>159</v>
@@ -4269,10 +4270,10 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B80" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C80" t="s">
         <v>243</v>
@@ -4669,10 +4670,10 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B100" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C100" t="s">
         <v>300</v>
@@ -7109,10 +7110,10 @@
     </row>
     <row r="222" spans="1:6">
       <c r="A222" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B222" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C222" t="s">
         <v>654</v>
@@ -7769,10 +7770,10 @@
     </row>
     <row r="255" spans="1:6">
       <c r="A255" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B255" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C255" t="s">
         <v>750</v>
@@ -7924,7 +7925,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F263"/>
+  <autoFilter ref="A1:F263" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>